<commit_message>
Base de données ajoutée
</commit_message>
<xml_diff>
--- a/NHAIRI_Planning_TPI.xlsx
+++ b/NHAIRI_Planning_TPI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>Préparation planning</t>
   </si>
@@ -63,15 +63,25 @@
   </si>
   <si>
     <t>Finnalisation</t>
+  </si>
+  <si>
+    <t>Planning TPI Ilias N'hairi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -340,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +390,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N32"/>
+  <dimension ref="B1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,80 +687,83 @@
     <col min="14" max="14" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="2:14" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16">
         <v>42864</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D4" s="17">
         <v>42865</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E4" s="17">
         <v>42866</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F4" s="17">
         <v>42867</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G4" s="17">
         <v>42871</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H4" s="17">
         <v>42872</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I4" s="17">
         <v>42873</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J4" s="17">
         <v>42874</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K4" s="17">
         <v>42878</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L4" s="18">
         <v>42879</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>0</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>1</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -761,15 +777,13 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -777,70 +791,57 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="5"/>
-      <c r="N7" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="D8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
-      <c r="N8" s="2" t="s">
-        <v>10</v>
+      <c r="N8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="F9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="5"/>
-      <c r="N9" s="3" t="s">
-        <v>11</v>
+      <c r="N9" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="20" t="s">
         <v>10</v>
       </c>
@@ -850,21 +851,20 @@
       <c r="I10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="20" t="s">
-        <v>10</v>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="N10" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>10</v>
+      </c>
       <c r="D11" s="20" t="s">
         <v>10</v>
       </c>
@@ -883,32 +883,46 @@
       <c r="I11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="4"/>
@@ -917,14 +931,18 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="J13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -934,7 +952,9 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
@@ -1157,20 +1177,36 @@
       <c r="K31" s="4"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="7"/>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="11"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:J2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fonction de lecture ajoutées
</commit_message>
<xml_diff>
--- a/NHAIRI_Planning_TPI.xlsx
+++ b/NHAIRI_Planning_TPI.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="09.05.2017" sheetId="1" r:id="rId1"/>
+    <sheet name="10.05.2017" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
   <si>
     <t>Préparation planning</t>
   </si>
@@ -676,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,4 +1211,546 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="12" width="15" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="2:14" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+    </row>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16">
+        <v>42864</v>
+      </c>
+      <c r="D4" s="17">
+        <v>42865</v>
+      </c>
+      <c r="E4" s="17">
+        <v>42866</v>
+      </c>
+      <c r="F4" s="17">
+        <v>42867</v>
+      </c>
+      <c r="G4" s="17">
+        <v>42871</v>
+      </c>
+      <c r="H4" s="17">
+        <v>42872</v>
+      </c>
+      <c r="I4" s="17">
+        <v>42873</v>
+      </c>
+      <c r="J4" s="17">
+        <v>42874</v>
+      </c>
+      <c r="K4" s="17">
+        <v>42878</v>
+      </c>
+      <c r="L4" s="18">
+        <v>42879</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="N8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="N9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="N10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="11"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>